<commit_message>
Create reference plots from all scripts, minor mods
</commit_message>
<xml_diff>
--- a/11-Parameters/LIONBeamLine-Params-Flat.xlsx
+++ b/11-Parameters/LIONBeamLine-Params-Flat.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/11-Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC65C5F-7DB2-F64B-BA11-D74A047C6E0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB015B40-C7B2-8E48-A62C-3111ED663BAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -737,7 +737,7 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:H4"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1018,7 +1018,7 @@
         <v>16</v>
       </c>
       <c r="F11" s="3">
-        <v>6.0339999999999998E-2</v>
+        <v>4.0340000000000001E-2</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>12</v>
@@ -1094,7 +1094,7 @@
         <v>16</v>
       </c>
       <c r="F14" s="7">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="G14" s="6" t="s">
         <v>12</v>
@@ -1290,7 +1290,7 @@
         <v>16</v>
       </c>
       <c r="F22" s="11">
-        <v>1.7285900000000001</v>
+        <v>1.7286520000000001</v>
       </c>
       <c r="G22" s="11" t="s">
         <v>12</v>
@@ -1314,7 +1314,7 @@
         <v>16</v>
       </c>
       <c r="F23" s="3">
-        <v>0.01</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Trying to implement flexible envelope calculations
</commit_message>
<xml_diff>
--- a/11-Parameters/LIONBeamLine-Params-Flat.xlsx
+++ b/11-Parameters/LIONBeamLine-Params-Flat.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/11-Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB015B40-C7B2-8E48-A62C-3111ED663BAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F4C4EF4-D961-4D48-9171-621EF7A3EEF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -397,19 +397,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -438,9 +435,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -478,7 +475,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -584,7 +581,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -726,7 +723,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -737,7 +734,7 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -753,100 +750,100 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="10" t="s">
+      <c r="F1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="12">
+      <c r="A2" s="9">
         <v>0</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="16">
+      <c r="A3" s="13">
         <v>0</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="F3" s="17">
-        <v>20</v>
-      </c>
-      <c r="G3" s="16" t="s">
+      <c r="F3" s="14">
+        <v>11</v>
+      </c>
+      <c r="G3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="16"/>
+      <c r="H3" s="13"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="13">
+      <c r="A4" s="10">
         <v>0</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="10">
         <v>0.5</v>
       </c>
-      <c r="G4" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="13"/>
+      <c r="G4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="10"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
@@ -975,7 +972,7 @@
       <c r="H9" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="J9" s="8" t="s">
+      <c r="J9" s="6" t="s">
         <v>36</v>
       </c>
     </row>
@@ -989,7 +986,7 @@
       <c r="C10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="12" t="s">
         <v>58</v>
       </c>
       <c r="E10" s="5" t="s">
@@ -1017,8 +1014,8 @@
       <c r="E11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="3">
-        <v>4.0340000000000001E-2</v>
+      <c r="F11">
+        <v>4.1180000000000001E-2</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>12</v>
@@ -1043,7 +1040,7 @@
       <c r="E12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="G12" s="3" t="s">
@@ -1080,50 +1077,50 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="6">
-        <v>1</v>
-      </c>
-      <c r="B14" s="6" t="s">
+      <c r="A14" s="3">
+        <v>1</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6" t="s">
+      <c r="D14" s="3"/>
+      <c r="E14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="3">
         <v>0</v>
       </c>
-      <c r="G14" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14" s="6" t="s">
+      <c r="G14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="6">
-        <v>1</v>
-      </c>
-      <c r="B15" s="6" t="s">
+      <c r="A15" s="3">
+        <v>1</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6" t="s">
+      <c r="D15" s="3"/>
+      <c r="E15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="3">
         <v>0.04</v>
       </c>
-      <c r="G15" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H15" s="6" t="s">
+      <c r="G15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" s="3" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1141,7 +1138,7 @@
       <c r="E16" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="3">
         <v>332</v>
       </c>
       <c r="G16" s="3" t="s">
@@ -1178,50 +1175,50 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="6">
-        <v>1</v>
-      </c>
-      <c r="B18" s="6" t="s">
+      <c r="A18" s="3">
+        <v>1</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6" t="s">
+      <c r="D18" s="3"/>
+      <c r="E18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F18" s="7">
-        <v>2.5770000000000001E-2</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H18" s="6" t="s">
+      <c r="F18" s="3">
+        <v>3.6953E-2</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="6">
-        <v>1</v>
-      </c>
-      <c r="B19" s="6" t="s">
+      <c r="A19" s="3">
+        <v>1</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6" t="s">
+      <c r="D19" s="3"/>
+      <c r="E19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="3">
         <v>0.02</v>
       </c>
-      <c r="G19" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H19" s="6" t="s">
+      <c r="G19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19" s="3" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1276,26 +1273,26 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="11">
-        <v>1</v>
-      </c>
-      <c r="B22" s="11" t="s">
+      <c r="A22" s="3">
+        <v>1</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11" t="s">
+      <c r="D22" s="3"/>
+      <c r="E22" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="11">
-        <v>1.7286520000000001</v>
-      </c>
-      <c r="G22" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H22" s="11" t="s">
+      <c r="F22" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H22" s="3" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>